<commit_message>
Rename dup columns on --oldAppend or --newAppend
</commit_message>
<xml_diff>
--- a/test1newAppend-expected.xlsx
+++ b/test1newAppend-expected.xlsx
@@ -595,12 +595,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>ID_1</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Fruit</t>
+          <t>Fruit_1</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -610,7 +610,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Color</t>
+          <t>Color_1</t>
         </is>
       </c>
     </row>

</xml_diff>